<commit_message>
Revert "Merge remote-tracking branch 'origin/presentatie' into presentatie"
This reverts commit e7e727f3b425882264f396850cc3ffdddc2e6d1d.
</commit_message>
<xml_diff>
--- a/Presentatie/2. Asset List Game-Lab Voorbeeld.xlsx
+++ b/Presentatie/2. Asset List Game-Lab Voorbeeld.xlsx
@@ -220,7 +220,7 @@
     <t>Hallo</t>
   </si>
   <si>
-    <t>Jood heil hitler</t>
+    <t>Jood</t>
   </si>
 </sst>
 </file>
@@ -705,7 +705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>

</xml_diff>